<commit_message>
add feature: get data from CMS, writer and customer review
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/outputArticles.xlsx
+++ b/src/test/resources/testdata/outputArticles.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study\repo\Maven-e2e-WPH\src\test\resources\testdata\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="122">
   <si>
     <t>id</t>
   </si>
@@ -392,7 +392,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -432,7 +431,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="2">
@@ -465,7 +464,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="292">
+  <cellXfs count="356">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -767,571 +766,763 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1610,19 +1801,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N113"/>
+  <dimension ref="A1:N161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" activeCellId="1" sqref="A43 L40"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="45.5703125"/>
-    <col min="2" max="2" customWidth="true" width="24.140625"/>
+    <col min="1" max="1" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1639,7 +1830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1649,11 +1840,11 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="N2" t="s" s="243">
+      <c r="N2" s="307" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:14">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -1663,11 +1854,11 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="N3" t="s" s="246">
+      <c r="N3" s="310" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:14">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -1677,11 +1868,11 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="N4" t="s" s="249">
+      <c r="N4" s="313" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:14">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -1691,11 +1882,11 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="N5" t="s" s="252">
+      <c r="N5" s="316" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:14">
       <c r="A6" s="13" t="s">
         <v>17</v>
       </c>
@@ -1705,11 +1896,11 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="N6" t="s" s="255">
+      <c r="N6" s="319" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:14">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -1719,11 +1910,11 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="N7" t="s" s="258">
+      <c r="N7" s="322" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:14">
       <c r="A8" s="17" t="s">
         <v>21</v>
       </c>
@@ -1733,271 +1924,271 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="N8" t="s" s="261">
+      <c r="N8" s="325" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:14">
       <c r="A9" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="N9" t="s" s="264">
+      <c r="N9" s="328" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:14">
       <c r="A10" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N10" t="s" s="267">
+      <c r="N10" s="331" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:14">
       <c r="A11" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="N11" t="s" s="270">
+      <c r="N11" s="334" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:14">
       <c r="A12" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="N12" t="s" s="273">
+      <c r="N12" s="337" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:14">
       <c r="A13" s="27" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="N13" t="s" s="276">
+      <c r="N13" s="340" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:14">
       <c r="A14" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="N14" t="s" s="279">
+      <c r="N14" s="343" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:14">
       <c r="A15" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="N15" t="s" s="282">
+      <c r="N15" s="346" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:14">
       <c r="A16" s="33" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="N16" t="s" s="285">
+      <c r="N16" s="349" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:14">
       <c r="A17" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="N17" t="s" s="288">
+      <c r="N17" s="352" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:14">
       <c r="A18" s="37" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="N18" t="s" s="291">
+      <c r="N18" s="355" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:14">
       <c r="A19" s="39" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="N19" t="s" s="198">
+      <c r="N19" s="265" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:14">
       <c r="A20" s="41" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="N20" t="s" s="201">
+      <c r="N20" s="268" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:14">
       <c r="A21" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="N21" t="s" s="204">
+      <c r="N21" s="271" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:14">
       <c r="A22" s="45" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="N22" t="s" s="207">
+      <c r="N22" s="274" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:14">
       <c r="A23" s="47" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="N23" t="s" s="210">
+      <c r="N23" s="277" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:14">
       <c r="A24" s="49" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="N24" t="s" s="213">
+      <c r="N24" s="280" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:14">
       <c r="A25" s="51" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="N25" t="s" s="216">
+      <c r="N25" s="283" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:14">
       <c r="A26" s="53" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="N26" t="s" s="219">
+      <c r="N26" s="286" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:14">
       <c r="A27" s="55" t="s">
         <v>59</v>
       </c>
       <c r="B27" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="N27" t="s" s="222">
+      <c r="N27" s="289" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:14">
       <c r="A28" s="57" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="N28" t="s" s="225">
+      <c r="N28" s="292" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:14">
       <c r="A29" s="59" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="N29" t="s" s="228">
+      <c r="N29" s="295" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:14">
       <c r="A30" s="61" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="N30" t="s" s="231">
+      <c r="N30" s="298" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:14">
       <c r="A31" s="63" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="N31" t="s" s="234">
+      <c r="N31" s="301" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:14">
       <c r="A32" s="65" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="N32" t="s" s="237">
+      <c r="N32" s="304" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2145,507 +2336,891 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="s" s="103">
+    <row r="51" spans="1:2">
+      <c r="A51" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B51" t="s" s="104">
+      <c r="B51" s="104" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="s" s="106">
+    <row r="52" spans="1:2">
+      <c r="A52" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B52" t="s" s="107">
+      <c r="B52" s="106" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="s" s="109">
+    <row r="53" spans="1:2">
+      <c r="A53" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="B53" t="s" s="110">
+      <c r="B53" s="108" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="s" s="112">
+    <row r="54" spans="1:2">
+      <c r="A54" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="B54" t="s" s="113">
+      <c r="B54" s="110" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="s" s="115">
+    <row r="55" spans="1:2">
+      <c r="A55" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="B55" t="s" s="116">
+      <c r="B55" s="112" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s" s="118">
+    <row r="56" spans="1:2">
+      <c r="A56" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="B56" t="s" s="119">
+      <c r="B56" s="114" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s" s="121">
+    <row r="57" spans="1:2">
+      <c r="A57" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="B57" t="s" s="122">
+      <c r="B57" s="116" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="124" t="s">
+      <c r="A58" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="B58" t="s" s="125">
+      <c r="B58" s="118" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="127">
+    <row r="59" spans="1:2">
+      <c r="A59" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="B59" t="s" s="128">
+      <c r="B59" s="120" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="s" s="130">
+    <row r="60" spans="1:2">
+      <c r="A60" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="B60" t="s" s="131">
+      <c r="B60" s="122" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="s" s="133">
+    <row r="61" spans="1:2">
+      <c r="A61" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="B61" t="s" s="134">
+      <c r="B61" s="124" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="s" s="136">
+    <row r="62" spans="1:2">
+      <c r="A62" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="B62" t="s" s="137">
+      <c r="B62" s="126" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="s" s="139">
+    <row r="63" spans="1:2">
+      <c r="A63" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="B63" t="s" s="140">
+      <c r="B63" s="128" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="s" s="142">
+    <row r="64" spans="1:2">
+      <c r="A64" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="B64" t="s" s="143">
+      <c r="B64" s="130" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" t="s" s="145">
+      <c r="A65" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="146" t="s">
+      <c r="B65" s="132" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="s" s="148">
+    <row r="66" spans="1:2">
+      <c r="A66" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="B66" t="s" s="149">
+      <c r="B66" s="134" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="s" s="151">
+    <row r="67" spans="1:2">
+      <c r="A67" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="B67" t="s" s="152">
+      <c r="B67" s="136" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="s" s="154">
+    <row r="68" spans="1:2">
+      <c r="A68" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="B68" t="s" s="155">
+      <c r="B68" s="138" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="s" s="157">
+    <row r="69" spans="1:2">
+      <c r="A69" s="139" t="s">
         <v>45</v>
       </c>
-      <c r="B69" t="s" s="158">
+      <c r="B69" s="140" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="s" s="160">
+    <row r="70" spans="1:2">
+      <c r="A70" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="B70" t="s" s="161">
+      <c r="B70" s="142" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="s" s="163">
+    <row r="71" spans="1:2">
+      <c r="A71" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="B71" t="s" s="164">
+      <c r="B71" s="144" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="s" s="166">
+    <row r="72" spans="1:2">
+      <c r="A72" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="B72" t="s" s="167">
+      <c r="B72" s="146" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="s" s="169">
+    <row r="73" spans="1:2">
+      <c r="A73" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="B73" t="s" s="170">
+      <c r="B73" s="148" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="172" t="s">
+      <c r="A74" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="B74" t="s" s="173">
+      <c r="B74" s="150" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="s" s="175">
+    <row r="75" spans="1:2">
+      <c r="A75" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="B75" t="s" s="176">
+      <c r="B75" s="152" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="s" s="178">
+    <row r="76" spans="1:2">
+      <c r="A76" s="153" t="s">
         <v>59</v>
       </c>
-      <c r="B76" t="s" s="179">
+      <c r="B76" s="154" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="s" s="181">
+    <row r="77" spans="1:2">
+      <c r="A77" s="155" t="s">
         <v>61</v>
       </c>
-      <c r="B77" t="s" s="182">
+      <c r="B77" s="156" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="s" s="184">
+    <row r="78" spans="1:2">
+      <c r="A78" s="157" t="s">
         <v>63</v>
       </c>
-      <c r="B78" t="s" s="185">
+      <c r="B78" s="158" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="s" s="187">
+    <row r="79" spans="1:2">
+      <c r="A79" s="159" t="s">
         <v>65</v>
       </c>
-      <c r="B79" t="s" s="188">
+      <c r="B79" s="160" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="s" s="190">
+    <row r="80" spans="1:2">
+      <c r="A80" s="161" t="s">
         <v>67</v>
       </c>
-      <c r="B80" t="s" s="191">
+      <c r="B80" s="162" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="s" s="193">
+    <row r="81" spans="1:2">
+      <c r="A81" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="B81" t="s" s="194">
+      <c r="B81" s="164" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" t="s" s="196">
+      <c r="A82" s="165" t="s">
         <v>71</v>
       </c>
-      <c r="B82" s="197" t="s">
+      <c r="B82" s="166" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="s" s="199">
+    <row r="83" spans="1:2">
+      <c r="A83" s="167" t="s">
         <v>73</v>
       </c>
-      <c r="B83" t="s" s="200">
+      <c r="B83" s="168" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="s" s="202">
+    <row r="84" spans="1:2">
+      <c r="A84" s="169" t="s">
         <v>74</v>
       </c>
-      <c r="B84" t="s" s="203">
+      <c r="B84" s="170" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="s" s="205">
+    <row r="85" spans="1:2">
+      <c r="A85" s="171" t="s">
         <v>76</v>
       </c>
-      <c r="B85" t="s" s="206">
+      <c r="B85" s="172" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="s" s="208">
+    <row r="86" spans="1:2">
+      <c r="A86" s="173" t="s">
         <v>78</v>
       </c>
-      <c r="B86" t="s" s="209">
+      <c r="B86" s="174" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="s" s="211">
+    <row r="87" spans="1:2">
+      <c r="A87" s="175" t="s">
         <v>80</v>
       </c>
-      <c r="B87" t="s" s="212">
+      <c r="B87" s="176" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="s" s="214">
+    <row r="88" spans="1:2">
+      <c r="A88" s="177" t="s">
         <v>82</v>
       </c>
-      <c r="B88" t="s" s="215">
+      <c r="B88" s="178" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="s" s="217">
+    <row r="89" spans="1:2">
+      <c r="A89" s="179" t="s">
         <v>84</v>
       </c>
-      <c r="B89" t="s" s="218">
+      <c r="B89" s="180" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="s" s="220">
+    <row r="90" spans="1:2">
+      <c r="A90" s="181" t="s">
         <v>86</v>
       </c>
-      <c r="B90" t="s" s="221">
+      <c r="B90" s="182" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="s" s="223">
+    <row r="91" spans="1:2">
+      <c r="A91" s="183" t="s">
         <v>88</v>
       </c>
-      <c r="B91" t="s" s="224">
+      <c r="B91" s="184" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="226" t="s">
+      <c r="A92" s="185" t="s">
         <v>90</v>
       </c>
-      <c r="B92" t="s" s="227">
+      <c r="B92" s="186" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="s" s="229">
+    <row r="93" spans="1:2">
+      <c r="A93" s="187" t="s">
         <v>92</v>
       </c>
-      <c r="B93" t="s" s="230">
+      <c r="B93" s="188" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="s" s="232">
+    <row r="94" spans="1:2">
+      <c r="A94" s="189" t="s">
         <v>94</v>
       </c>
-      <c r="B94" t="s" s="233">
+      <c r="B94" s="190" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="s" s="235">
+    <row r="95" spans="1:2">
+      <c r="A95" s="191" t="s">
         <v>96</v>
       </c>
-      <c r="B95" t="s" s="236">
+      <c r="B95" s="192" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="s" s="238">
+    <row r="96" spans="1:2">
+      <c r="A96" s="193" t="s">
         <v>107</v>
       </c>
-      <c r="B96" t="s" s="239">
+      <c r="B96" s="194" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" t="s" s="241">
+    <row r="97" spans="1:2">
+      <c r="A97" s="195" t="s">
         <v>98</v>
       </c>
-      <c r="B97" t="s" s="242">
+      <c r="B97" s="196" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="s" s="244">
+    <row r="98" spans="1:2">
+      <c r="A98" s="197" t="s">
         <v>100</v>
       </c>
-      <c r="B98" t="s" s="245">
+      <c r="B98" s="198" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="s" s="247">
+    <row r="99" spans="1:2">
+      <c r="A99" s="199" t="s">
         <v>102</v>
       </c>
-      <c r="B99" t="s" s="248">
+      <c r="B99" s="200" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="s" s="250">
+    <row r="100" spans="1:2">
+      <c r="A100" s="201" t="s">
         <v>104</v>
       </c>
-      <c r="B100" t="s" s="251">
+      <c r="B100" s="202" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="s" s="253">
+    <row r="101" spans="1:2">
+      <c r="A101" s="203" t="s">
         <v>109</v>
       </c>
-      <c r="B101" t="s" s="254">
+      <c r="B101" s="204" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" t="s" s="256">
+    <row r="102" spans="1:2">
+      <c r="A102" s="205" t="s">
         <v>110</v>
       </c>
-      <c r="B102" t="s" s="257">
+      <c r="B102" s="206" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" t="s" s="259">
+    <row r="103" spans="1:2">
+      <c r="A103" s="207" t="s">
         <v>111</v>
       </c>
-      <c r="B103" t="s" s="260">
+      <c r="B103" s="208" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" t="s" s="262">
+    <row r="104" spans="1:2">
+      <c r="A104" s="209" t="s">
         <v>112</v>
       </c>
-      <c r="B104" t="s" s="263">
+      <c r="B104" s="210" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" t="s" s="265">
+    <row r="105" spans="1:2">
+      <c r="A105" s="211" t="s">
         <v>113</v>
       </c>
-      <c r="B105" t="s" s="266">
+      <c r="B105" s="212" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" t="s" s="268">
+    <row r="106" spans="1:2">
+      <c r="A106" s="213" t="s">
         <v>114</v>
       </c>
-      <c r="B106" t="s" s="269">
+      <c r="B106" s="214" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" t="s" s="271">
+    <row r="107" spans="1:2">
+      <c r="A107" s="215" t="s">
         <v>115</v>
       </c>
-      <c r="B107" t="s" s="272">
+      <c r="B107" s="216" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" t="s" s="274">
+    <row r="108" spans="1:2">
+      <c r="A108" s="217" t="s">
         <v>116</v>
       </c>
-      <c r="B108" t="s" s="275">
+      <c r="B108" s="218" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" t="s" s="277">
+    <row r="109" spans="1:2">
+      <c r="A109" s="219" t="s">
         <v>117</v>
       </c>
-      <c r="B109" t="s" s="278">
+      <c r="B109" s="220" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" t="s" s="280">
+    <row r="110" spans="1:2">
+      <c r="A110" s="221" t="s">
         <v>118</v>
       </c>
-      <c r="B110" t="s" s="281">
+      <c r="B110" s="222" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" t="s" s="283">
+    <row r="111" spans="1:2">
+      <c r="A111" s="223" t="s">
         <v>119</v>
       </c>
-      <c r="B111" t="s" s="284">
+      <c r="B111" s="224" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" t="s" s="286">
+    <row r="112" spans="1:2">
+      <c r="A112" s="225" t="s">
         <v>120</v>
       </c>
-      <c r="B112" t="s" s="287">
+      <c r="B112" s="226" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" t="s" s="289">
+    <row r="113" spans="1:2">
+      <c r="A113" s="227" t="s">
         <v>121</v>
       </c>
-      <c r="B113" t="s" s="290">
+      <c r="B113" s="228" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="229" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="230" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="231" t="s">
+        <v>21</v>
+      </c>
+      <c r="B115" s="232" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="233" t="s">
+        <v>23</v>
+      </c>
+      <c r="B116" s="234" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="235" t="s">
+        <v>25</v>
+      </c>
+      <c r="B117" s="236" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="237" t="s">
+        <v>27</v>
+      </c>
+      <c r="B118" s="238" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="239" t="s">
+        <v>29</v>
+      </c>
+      <c r="B119" s="240" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="241" t="s">
+        <v>31</v>
+      </c>
+      <c r="B120" s="242" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="243" t="s">
+        <v>33</v>
+      </c>
+      <c r="B121" s="244" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="245" t="s">
+        <v>35</v>
+      </c>
+      <c r="B122" s="246" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="247" t="s">
+        <v>37</v>
+      </c>
+      <c r="B123" s="248" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="249" t="s">
+        <v>39</v>
+      </c>
+      <c r="B124" s="250" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="251" t="s">
+        <v>41</v>
+      </c>
+      <c r="B125" s="252" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="253" t="s">
+        <v>43</v>
+      </c>
+      <c r="B126" s="254" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="255" t="s">
+        <v>45</v>
+      </c>
+      <c r="B127" s="256" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="257" t="s">
+        <v>47</v>
+      </c>
+      <c r="B128" s="258" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="259" t="s">
+        <v>49</v>
+      </c>
+      <c r="B129" s="260" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="261" t="s">
+        <v>51</v>
+      </c>
+      <c r="B130" s="262" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="263" t="s">
+        <v>53</v>
+      </c>
+      <c r="B131" s="264" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="266" t="s">
+        <v>55</v>
+      </c>
+      <c r="B132" s="267" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="269" t="s">
+        <v>57</v>
+      </c>
+      <c r="B133" s="270" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="272" t="s">
+        <v>59</v>
+      </c>
+      <c r="B134" s="273" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="275" t="s">
+        <v>61</v>
+      </c>
+      <c r="B135" s="276" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="278" t="s">
+        <v>63</v>
+      </c>
+      <c r="B136" s="279" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="281" t="s">
+        <v>65</v>
+      </c>
+      <c r="B137" s="282" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="284" t="s">
+        <v>67</v>
+      </c>
+      <c r="B138" s="285" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="287" t="s">
+        <v>69</v>
+      </c>
+      <c r="B139" s="288" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="290" t="s">
+        <v>71</v>
+      </c>
+      <c r="B140" s="291" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="293" t="s">
+        <v>73</v>
+      </c>
+      <c r="B141" s="294" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="296" t="s">
+        <v>74</v>
+      </c>
+      <c r="B142" s="297" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="299" t="s">
+        <v>76</v>
+      </c>
+      <c r="B143" s="300" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="302" t="s">
+        <v>78</v>
+      </c>
+      <c r="B144" s="303" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="305" t="s">
+        <v>80</v>
+      </c>
+      <c r="B145" s="306" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="308" t="s">
+        <v>82</v>
+      </c>
+      <c r="B146" s="309" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="311" t="s">
+        <v>84</v>
+      </c>
+      <c r="B147" s="312" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="314" t="s">
+        <v>86</v>
+      </c>
+      <c r="B148" s="315" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="317" t="s">
+        <v>88</v>
+      </c>
+      <c r="B149" s="318" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="320" t="s">
+        <v>90</v>
+      </c>
+      <c r="B150" s="321" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="323" t="s">
+        <v>92</v>
+      </c>
+      <c r="B151" s="324" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="326" t="s">
+        <v>94</v>
+      </c>
+      <c r="B152" s="327" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="329" t="s">
+        <v>96</v>
+      </c>
+      <c r="B153" s="330" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="332" t="s">
+        <v>98</v>
+      </c>
+      <c r="B154" s="333" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="335" t="s">
+        <v>100</v>
+      </c>
+      <c r="B155" s="336" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="338" t="s">
+        <v>102</v>
+      </c>
+      <c r="B156" s="339" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="341" t="s">
+        <v>104</v>
+      </c>
+      <c r="B157" s="342" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="344" t="s">
+        <v>109</v>
+      </c>
+      <c r="B158" s="345" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="347" t="s">
+        <v>110</v>
+      </c>
+      <c r="B159" s="348" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="350" t="s">
+        <v>111</v>
+      </c>
+      <c r="B160" s="351" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="353" t="s">
+        <v>112</v>
+      </c>
+      <c r="B161" s="354" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2667,8 +3242,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="45.5703125"/>
-    <col min="2" max="2" customWidth="true" width="24.140625"/>
+    <col min="1" max="1" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
add sample services for ibh
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/outputArticles.xlsx
+++ b/src/test/resources/testdata/outputArticles.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="431">
   <si>
     <t>ID</t>
   </si>
@@ -1071,6 +1071,243 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>https://yeti-cloud.com/yeti/main/writers/edit/214</t>
+  </si>
+  <si>
+    <t>https://yeti-cloud.com/yeti/main/writers/edit/215</t>
+  </si>
+  <si>
+    <t>https://yeti-cloud.com/yeti/main/writers/edit/216</t>
+  </si>
+  <si>
+    <t>https://yeti-cloud.com/yeti/main/writers/edit/217</t>
+  </si>
+  <si>
+    <t>https://yeti-cloud.com/yeti/main/writers/edit/218</t>
+  </si>
+  <si>
+    <t>https://yeti-cloud.com/yeti/main/writers/edit/219</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/264</t>
+  </si>
+  <si>
+    <t>/samples/essay/gender-studies</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/265</t>
+  </si>
+  <si>
+    <t>/samples/essay/persuasive-essay</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/266</t>
+  </si>
+  <si>
+    <t>/samples/essay/mba-application</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/267</t>
+  </si>
+  <si>
+    <t>/samples/essay/anthropology</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/268</t>
+  </si>
+  <si>
+    <t>/samples/essay/criminal-law</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/269</t>
+  </si>
+  <si>
+    <t>/samples/discussion-post/health-care</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/270</t>
+  </si>
+  <si>
+    <t>/discussion-post/history</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/271</t>
+  </si>
+  <si>
+    <t>/samples/discussion-post/statistics</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/272</t>
+  </si>
+  <si>
+    <t>/samples/critical-thinking/criminal-law</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/273</t>
+  </si>
+  <si>
+    <t>/samples/critical-thinking/culture-and-society</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/274</t>
+  </si>
+  <si>
+    <t>/samples/term-paper/criminal-law</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/275</t>
+  </si>
+  <si>
+    <t>/samples/homework/statistics</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/276</t>
+  </si>
+  <si>
+    <t>/samples/research-paper/apa</t>
+  </si>
+  <si>
+    <t>/samples/research-paper/gun-control</t>
+  </si>
+  <si>
+    <t>/samples/research-paper/business-managment</t>
+  </si>
+  <si>
+    <t>/samples/research-proposal/phd</t>
+  </si>
+  <si>
+    <t>/samples/research-proposal/mla</t>
+  </si>
+  <si>
+    <t>/samples/personal-statement/medicine</t>
+  </si>
+  <si>
+    <t>/samples/powerpoint-presentation/powerpoint-presentation-apa</t>
+  </si>
+  <si>
+    <t>/samples/speech/graduation</t>
+  </si>
+  <si>
+    <t>/samples/speech/high-school</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/277</t>
+  </si>
+  <si>
+    <t>/samples/lab-report/spectrophotometry-lab</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/278</t>
+  </si>
+  <si>
+    <t>/samples/lab-report/chemistry</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/279</t>
+  </si>
+  <si>
+    <t>/samples/lab-report/physics</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/280</t>
+  </si>
+  <si>
+    <t>/samples/lab-report/biology</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/281</t>
+  </si>
+  <si>
+    <t>/samples/lab-report/statistics</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/282</t>
+  </si>
+  <si>
+    <t>/samples/lesson-plan/education</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/283</t>
+  </si>
+  <si>
+    <t>/samples/nursing-plan/nursing</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/284</t>
+  </si>
+  <si>
+    <t>/samples/epq-essay/essay</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/285</t>
+  </si>
+  <si>
+    <t>/samples/epq-presentation/presentation</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/286</t>
+  </si>
+  <si>
+    <t>/samples/question-answer/psychology</t>
+  </si>
+  <si>
+    <t>/test-new-service-page</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/articles/save</t>
+  </si>
+  <si>
+    <t>/NewServicePageTest</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/287</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/288</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/289</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/290</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/291</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/292</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/293</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/294</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/295</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/296</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/samples/edit/297</t>
+  </si>
+  <si>
+    <t>/Servicepage.test2</t>
+  </si>
+  <si>
+    <t>/NEWSERVICEPAGE</t>
+  </si>
+  <si>
+    <t>/sample-hien</t>
+  </si>
+  <si>
+    <t>/samples-list</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/articles/edit/195</t>
   </si>
 </sst>
 </file>
@@ -1714,10 +1951,1060 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1013">
+  <cellXfs count="1363">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
@@ -5069,7 +6356,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E637"/>
+  <dimension ref="A1:E839"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -5105,7 +6392,7 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="488" t="s">
+      <c r="C2" s="1230" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5116,7 +6403,7 @@
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="490" t="s">
+      <c r="C3" s="1232" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5127,7 +6414,7 @@
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="492" t="s">
+      <c r="C4" s="1234" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5138,7 +6425,7 @@
       <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="494" t="s">
+      <c r="C5" s="1236" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5149,7 +6436,7 @@
       <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="496" t="s">
+      <c r="C6" s="1238" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5160,7 +6447,7 @@
       <c r="B7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="498" t="s">
+      <c r="C7" s="1240" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5171,7 +6458,7 @@
       <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="500" t="s">
+      <c r="C8" s="1242" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5182,7 +6469,7 @@
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="502" t="s">
+      <c r="C9" s="1244" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5193,7 +6480,7 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="504" t="s">
+      <c r="C10" s="1246" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5204,7 +6491,7 @@
       <c r="B11" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="506" t="s">
+      <c r="C11" s="1248" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5215,7 +6502,7 @@
       <c r="B12" s="996" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="508" t="s">
+      <c r="C12" s="1250" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5226,7 +6513,7 @@
       <c r="B13" s="998" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="510" t="s">
+      <c r="C13" s="1252" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5237,7 +6524,7 @@
       <c r="B14" s="1000" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="512" t="s">
+      <c r="C14" s="1254" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5248,7 +6535,7 @@
       <c r="B15" s="1002" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="514" t="s">
+      <c r="C15" s="1256" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5259,7 +6546,7 @@
       <c r="B16" s="1004" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="516" t="s">
+      <c r="C16" s="1258" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5270,7 +6557,7 @@
       <c r="B17" s="1006" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="518" t="s">
+      <c r="C17" s="1260" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5281,7 +6568,7 @@
       <c r="B18" s="1008" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="520" t="s">
+      <c r="C18" s="1262" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5292,7 +6579,7 @@
       <c r="B19" s="1010" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="522" t="s">
+      <c r="C19" s="1264" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5303,7 +6590,7 @@
       <c r="B20" s="1012" t="s">
         <v>351</v>
       </c>
-      <c r="C20" s="524" t="s">
+      <c r="C20" s="1266" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5311,8 +6598,10 @@
       <c r="A21" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="526" t="s">
+      <c r="B21" s="1020" t="s">
+        <v>359</v>
+      </c>
+      <c r="C21" s="1268" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5320,8 +6609,10 @@
       <c r="A22" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="528" t="s">
+      <c r="B22" s="1022" t="s">
+        <v>361</v>
+      </c>
+      <c r="C22" s="1270" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5329,8 +6620,10 @@
       <c r="A23" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="530" t="s">
+      <c r="B23" s="1024" t="s">
+        <v>363</v>
+      </c>
+      <c r="C23" s="1272" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5338,8 +6631,10 @@
       <c r="A24" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="532" t="s">
+      <c r="B24" s="1026" t="s">
+        <v>365</v>
+      </c>
+      <c r="C24" s="1274" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5347,8 +6642,10 @@
       <c r="A25" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="534" t="s">
+      <c r="B25" s="1028" t="s">
+        <v>367</v>
+      </c>
+      <c r="C25" s="1276" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5356,8 +6653,10 @@
       <c r="A26" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="536" t="s">
+      <c r="B26" s="1030" t="s">
+        <v>369</v>
+      </c>
+      <c r="C26" s="1278" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5365,8 +6664,10 @@
       <c r="A27" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="538" t="s">
+      <c r="B27" s="1032" t="s">
+        <v>371</v>
+      </c>
+      <c r="C27" s="1280" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5374,8 +6675,10 @@
       <c r="A28" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="540" t="s">
+      <c r="B28" s="1034" t="s">
+        <v>373</v>
+      </c>
+      <c r="C28" s="1282" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5383,8 +6686,10 @@
       <c r="A29" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="542" t="s">
+      <c r="B29" s="1036" t="s">
+        <v>375</v>
+      </c>
+      <c r="C29" s="1284" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5392,7 +6697,9 @@
       <c r="A30" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="1038" t="s">
+        <v>377</v>
+      </c>
       <c r="C30" s="544" t="s">
         <v>17</v>
       </c>
@@ -5401,7 +6708,9 @@
       <c r="A31" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="1040" t="s">
+        <v>379</v>
+      </c>
       <c r="C31" s="546" t="s">
         <v>17</v>
       </c>
@@ -5410,7 +6719,9 @@
       <c r="A32" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="1042" t="s">
+        <v>381</v>
+      </c>
       <c r="C32" s="548" t="s">
         <v>17</v>
       </c>
@@ -5419,7 +6730,9 @@
       <c r="A33" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="1044" t="s">
+        <v>383</v>
+      </c>
       <c r="C33" s="550" t="s">
         <v>17</v>
       </c>
@@ -5428,7 +6741,9 @@
       <c r="A34" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="1046" t="s">
+        <v>384</v>
+      </c>
       <c r="C34" s="552" t="s">
         <v>17</v>
       </c>
@@ -5437,7 +6752,9 @@
       <c r="A35" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="1048" t="s">
+        <v>385</v>
+      </c>
       <c r="C35" s="554" t="s">
         <v>17</v>
       </c>
@@ -5446,7 +6763,9 @@
       <c r="A36" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="1050" t="s">
+        <v>386</v>
+      </c>
       <c r="C36" s="556" t="s">
         <v>17</v>
       </c>
@@ -5455,7 +6774,9 @@
       <c r="A37" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="1052" t="s">
+        <v>387</v>
+      </c>
       <c r="C37" s="558" t="s">
         <v>17</v>
       </c>
@@ -5464,7 +6785,9 @@
       <c r="A38" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="1054" t="s">
+        <v>388</v>
+      </c>
       <c r="C38" s="560" t="s">
         <v>17</v>
       </c>
@@ -5473,7 +6796,9 @@
       <c r="A39" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="1056" t="s">
+        <v>389</v>
+      </c>
       <c r="C39" s="562" t="s">
         <v>17</v>
       </c>
@@ -5482,7 +6807,9 @@
       <c r="A40" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="1058" t="s">
+        <v>390</v>
+      </c>
       <c r="C40" s="564" t="s">
         <v>17</v>
       </c>
@@ -5491,7 +6818,9 @@
       <c r="A41" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="1060" t="s">
+        <v>359</v>
+      </c>
       <c r="C41" s="566" t="s">
         <v>17</v>
       </c>
@@ -5500,7 +6829,9 @@
       <c r="A42" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="1062" t="s">
+        <v>361</v>
+      </c>
       <c r="C42" s="568" t="s">
         <v>17</v>
       </c>
@@ -5509,7 +6840,9 @@
       <c r="A43" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="1064" t="s">
+        <v>363</v>
+      </c>
       <c r="C43" s="570" t="s">
         <v>17</v>
       </c>
@@ -5518,7 +6851,9 @@
       <c r="A44" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="1066" t="s">
+        <v>365</v>
+      </c>
       <c r="C44" s="572" t="s">
         <v>17</v>
       </c>
@@ -5527,7 +6862,9 @@
       <c r="A45" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="1068" t="s">
+        <v>367</v>
+      </c>
       <c r="C45" s="574" t="s">
         <v>17</v>
       </c>
@@ -5536,7 +6873,9 @@
       <c r="A46" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="1070" t="s">
+        <v>369</v>
+      </c>
       <c r="C46" s="576" t="s">
         <v>17</v>
       </c>
@@ -5545,7 +6884,9 @@
       <c r="A47" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="1072" t="s">
+        <v>371</v>
+      </c>
       <c r="C47" s="578" t="s">
         <v>17</v>
       </c>
@@ -5554,6 +6895,9 @@
       <c r="A48" s="60" t="s">
         <v>53</v>
       </c>
+      <c r="B48" t="s" s="1074">
+        <v>373</v>
+      </c>
       <c r="C48" s="580" t="s">
         <v>17</v>
       </c>
@@ -5562,6 +6906,9 @@
       <c r="A49" s="61" t="s">
         <v>54</v>
       </c>
+      <c r="B49" t="s" s="1156">
+        <v>375</v>
+      </c>
       <c r="C49" s="582" t="s">
         <v>17</v>
       </c>
@@ -5570,6 +6917,9 @@
       <c r="A50" s="62" t="s">
         <v>55</v>
       </c>
+      <c r="B50" t="s" s="1158">
+        <v>377</v>
+      </c>
       <c r="C50" s="584" t="s">
         <v>17</v>
       </c>
@@ -5578,6 +6928,9 @@
       <c r="A51" s="63" t="s">
         <v>56</v>
       </c>
+      <c r="B51" t="s" s="1160">
+        <v>379</v>
+      </c>
       <c r="C51" s="586" t="s">
         <v>17</v>
       </c>
@@ -5586,6 +6939,9 @@
       <c r="A52" s="64" t="s">
         <v>57</v>
       </c>
+      <c r="B52" t="s" s="1162">
+        <v>381</v>
+      </c>
       <c r="C52" s="588" t="s">
         <v>17</v>
       </c>
@@ -5594,6 +6950,9 @@
       <c r="A53" s="65" t="s">
         <v>58</v>
       </c>
+      <c r="B53" t="s" s="1164">
+        <v>383</v>
+      </c>
       <c r="C53" s="590" t="s">
         <v>17</v>
       </c>
@@ -5602,6 +6961,9 @@
       <c r="A54" s="66" t="s">
         <v>59</v>
       </c>
+      <c r="B54" t="s" s="1166">
+        <v>384</v>
+      </c>
       <c r="C54" s="592" t="s">
         <v>17</v>
       </c>
@@ -5610,6 +6972,9 @@
       <c r="A55" s="67" t="s">
         <v>60</v>
       </c>
+      <c r="B55" t="s" s="1168">
+        <v>385</v>
+      </c>
       <c r="C55" s="594" t="s">
         <v>17</v>
       </c>
@@ -5618,6 +6983,9 @@
       <c r="A56" s="68" t="s">
         <v>61</v>
       </c>
+      <c r="B56" t="s" s="1170">
+        <v>386</v>
+      </c>
       <c r="C56" s="596" t="s">
         <v>17</v>
       </c>
@@ -5626,6 +6994,9 @@
       <c r="A57" s="69" t="s">
         <v>62</v>
       </c>
+      <c r="B57" t="s" s="1172">
+        <v>387</v>
+      </c>
       <c r="C57" s="598" t="s">
         <v>17</v>
       </c>
@@ -5634,6 +7005,9 @@
       <c r="A58" s="70" t="s">
         <v>63</v>
       </c>
+      <c r="B58" t="s" s="1174">
+        <v>388</v>
+      </c>
       <c r="C58" s="600" t="s">
         <v>17</v>
       </c>
@@ -5642,6 +7016,9 @@
       <c r="A59" s="71" t="s">
         <v>64</v>
       </c>
+      <c r="B59" t="s" s="1176">
+        <v>389</v>
+      </c>
       <c r="C59" s="602" t="s">
         <v>17</v>
       </c>
@@ -5650,6 +7027,9 @@
       <c r="A60" s="72" t="s">
         <v>65</v>
       </c>
+      <c r="B60" t="s" s="1178">
+        <v>390</v>
+      </c>
       <c r="C60" s="604" t="s">
         <v>17</v>
       </c>
@@ -5658,6 +7038,9 @@
       <c r="A61" s="73" t="s">
         <v>66</v>
       </c>
+      <c r="B61" t="s" s="1180">
+        <v>391</v>
+      </c>
       <c r="C61" s="606" t="s">
         <v>17</v>
       </c>
@@ -5666,6 +7049,9 @@
       <c r="A62" s="74" t="s">
         <v>67</v>
       </c>
+      <c r="B62" t="s" s="1182">
+        <v>393</v>
+      </c>
       <c r="C62" s="608" t="s">
         <v>17</v>
       </c>
@@ -5674,6 +7060,9 @@
       <c r="A63" s="75" t="s">
         <v>68</v>
       </c>
+      <c r="B63" t="s" s="1184">
+        <v>395</v>
+      </c>
       <c r="C63" s="610" t="s">
         <v>17</v>
       </c>
@@ -5682,6 +7071,9 @@
       <c r="A64" s="76" t="s">
         <v>69</v>
       </c>
+      <c r="B64" t="s" s="1186">
+        <v>397</v>
+      </c>
       <c r="C64" s="612" t="s">
         <v>17</v>
       </c>
@@ -5690,6 +7082,9 @@
       <c r="A65" s="77" t="s">
         <v>70</v>
       </c>
+      <c r="B65" t="s" s="1188">
+        <v>399</v>
+      </c>
       <c r="C65" s="614" t="s">
         <v>17</v>
       </c>
@@ -5698,6 +7093,9 @@
       <c r="A66" s="78" t="s">
         <v>71</v>
       </c>
+      <c r="B66" t="s" s="1190">
+        <v>401</v>
+      </c>
       <c r="C66" s="616" t="s">
         <v>17</v>
       </c>
@@ -5706,6 +7104,9 @@
       <c r="A67" s="79" t="s">
         <v>72</v>
       </c>
+      <c r="B67" t="s" s="1192">
+        <v>403</v>
+      </c>
       <c r="C67" s="618" t="s">
         <v>17</v>
       </c>
@@ -5714,6 +7115,9 @@
       <c r="A68" s="80" t="s">
         <v>73</v>
       </c>
+      <c r="B68" t="s" s="1194">
+        <v>405</v>
+      </c>
       <c r="C68" s="620" t="s">
         <v>17</v>
       </c>
@@ -5722,6 +7126,9 @@
       <c r="A69" s="81" t="s">
         <v>74</v>
       </c>
+      <c r="B69" t="s" s="1196">
+        <v>407</v>
+      </c>
       <c r="C69" s="622" t="s">
         <v>17</v>
       </c>
@@ -5730,6 +7137,9 @@
       <c r="A70" s="82" t="s">
         <v>75</v>
       </c>
+      <c r="B70" t="s" s="1198">
+        <v>409</v>
+      </c>
       <c r="C70" s="624" t="s">
         <v>17</v>
       </c>
@@ -5738,6 +7148,9 @@
       <c r="A71" s="83" t="s">
         <v>76</v>
       </c>
+      <c r="B71" t="s" s="1200">
+        <v>411</v>
+      </c>
       <c r="C71" s="626" t="s">
         <v>17</v>
       </c>
@@ -5746,6 +7159,9 @@
       <c r="A72" s="84" t="s">
         <v>77</v>
       </c>
+      <c r="B72" t="s" s="1202">
+        <v>412</v>
+      </c>
       <c r="C72" s="628" t="s">
         <v>17</v>
       </c>
@@ -5754,6 +7170,9 @@
       <c r="A73" s="85" t="s">
         <v>78</v>
       </c>
+      <c r="B73" t="s" s="1204">
+        <v>414</v>
+      </c>
       <c r="C73" s="630" t="s">
         <v>17</v>
       </c>
@@ -5762,6 +7181,9 @@
       <c r="A74" s="86" t="s">
         <v>79</v>
       </c>
+      <c r="B74" t="s" s="1286">
+        <v>359</v>
+      </c>
       <c r="C74" s="632" t="s">
         <v>17</v>
       </c>
@@ -5770,6 +7192,9 @@
       <c r="A75" s="87" t="s">
         <v>80</v>
       </c>
+      <c r="B75" t="s" s="1288">
+        <v>361</v>
+      </c>
       <c r="C75" s="634" t="s">
         <v>17</v>
       </c>
@@ -5778,6 +7203,9 @@
       <c r="A76" s="88" t="s">
         <v>81</v>
       </c>
+      <c r="B76" t="s" s="1290">
+        <v>363</v>
+      </c>
       <c r="C76" s="636" t="s">
         <v>17</v>
       </c>
@@ -5786,6 +7214,9 @@
       <c r="A77" s="89" t="s">
         <v>82</v>
       </c>
+      <c r="B77" t="s" s="1292">
+        <v>365</v>
+      </c>
       <c r="C77" s="638" t="s">
         <v>17</v>
       </c>
@@ -5794,6 +7225,9 @@
       <c r="A78" s="90" t="s">
         <v>83</v>
       </c>
+      <c r="B78" t="s" s="1294">
+        <v>367</v>
+      </c>
       <c r="C78" s="640" t="s">
         <v>17</v>
       </c>
@@ -5802,6 +7236,9 @@
       <c r="A79" s="91" t="s">
         <v>84</v>
       </c>
+      <c r="B79" t="s" s="1296">
+        <v>369</v>
+      </c>
       <c r="C79" s="642" t="s">
         <v>17</v>
       </c>
@@ -5810,6 +7247,9 @@
       <c r="A80" s="92" t="s">
         <v>85</v>
       </c>
+      <c r="B80" t="s" s="1298">
+        <v>371</v>
+      </c>
       <c r="C80" s="644" t="s">
         <v>17</v>
       </c>
@@ -5818,6 +7258,9 @@
       <c r="A81" s="93" t="s">
         <v>86</v>
       </c>
+      <c r="B81" t="s" s="1300">
+        <v>373</v>
+      </c>
       <c r="C81" s="646" t="s">
         <v>17</v>
       </c>
@@ -5826,6 +7269,9 @@
       <c r="A82" s="94" t="s">
         <v>87</v>
       </c>
+      <c r="B82" t="s" s="1302">
+        <v>375</v>
+      </c>
       <c r="C82" s="648" t="s">
         <v>17</v>
       </c>
@@ -5834,6 +7280,9 @@
       <c r="A83" s="95" t="s">
         <v>88</v>
       </c>
+      <c r="B83" t="s" s="1304">
+        <v>377</v>
+      </c>
       <c r="C83" s="650" t="s">
         <v>17</v>
       </c>
@@ -5842,6 +7291,9 @@
       <c r="A84" s="96" t="s">
         <v>89</v>
       </c>
+      <c r="B84" t="s" s="1306">
+        <v>379</v>
+      </c>
       <c r="C84" s="652" t="s">
         <v>17</v>
       </c>
@@ -5850,6 +7302,9 @@
       <c r="A85" s="97" t="s">
         <v>90</v>
       </c>
+      <c r="B85" t="s" s="1308">
+        <v>381</v>
+      </c>
       <c r="C85" s="654" t="s">
         <v>17</v>
       </c>
@@ -5858,6 +7313,9 @@
       <c r="A86" s="98" t="s">
         <v>91</v>
       </c>
+      <c r="B86" t="s" s="1310">
+        <v>383</v>
+      </c>
       <c r="C86" s="656" t="s">
         <v>17</v>
       </c>
@@ -5866,6 +7324,9 @@
       <c r="A87" s="99" t="s">
         <v>92</v>
       </c>
+      <c r="B87" t="s" s="1312">
+        <v>384</v>
+      </c>
       <c r="C87" s="658" t="s">
         <v>17</v>
       </c>
@@ -5874,6 +7335,9 @@
       <c r="A88" s="100" t="s">
         <v>93</v>
       </c>
+      <c r="B88" t="s" s="1314">
+        <v>385</v>
+      </c>
       <c r="C88" s="660" t="s">
         <v>17</v>
       </c>
@@ -5882,6 +7346,9 @@
       <c r="A89" s="101" t="s">
         <v>94</v>
       </c>
+      <c r="B89" t="s" s="1316">
+        <v>386</v>
+      </c>
       <c r="C89" s="662" t="s">
         <v>17</v>
       </c>
@@ -5890,6 +7357,9 @@
       <c r="A90" s="102" t="s">
         <v>95</v>
       </c>
+      <c r="B90" t="s" s="1318">
+        <v>387</v>
+      </c>
       <c r="C90" s="664" t="s">
         <v>17</v>
       </c>
@@ -5898,6 +7368,9 @@
       <c r="A91" s="103" t="s">
         <v>96</v>
       </c>
+      <c r="B91" t="s" s="1320">
+        <v>388</v>
+      </c>
       <c r="C91" s="666" t="s">
         <v>17</v>
       </c>
@@ -5906,6 +7379,9 @@
       <c r="A92" s="104" t="s">
         <v>97</v>
       </c>
+      <c r="B92" t="s" s="1322">
+        <v>389</v>
+      </c>
       <c r="C92" s="668" t="s">
         <v>17</v>
       </c>
@@ -5914,6 +7390,9 @@
       <c r="A93" s="105" t="s">
         <v>98</v>
       </c>
+      <c r="B93" t="s" s="1324">
+        <v>390</v>
+      </c>
       <c r="C93" s="670" t="s">
         <v>17</v>
       </c>
@@ -5922,6 +7401,9 @@
       <c r="A94" s="106" t="s">
         <v>99</v>
       </c>
+      <c r="B94" t="s" s="1326">
+        <v>391</v>
+      </c>
       <c r="C94" s="672" t="s">
         <v>17</v>
       </c>
@@ -5930,6 +7412,9 @@
       <c r="A95" s="107" t="s">
         <v>100</v>
       </c>
+      <c r="B95" t="s" s="1328">
+        <v>393</v>
+      </c>
       <c r="C95" s="674" t="s">
         <v>17</v>
       </c>
@@ -5938,6 +7423,9 @@
       <c r="A96" s="108" t="s">
         <v>101</v>
       </c>
+      <c r="B96" t="s" s="1330">
+        <v>395</v>
+      </c>
       <c r="C96" s="676" t="s">
         <v>17</v>
       </c>
@@ -5946,6 +7434,9 @@
       <c r="A97" s="109" t="s">
         <v>102</v>
       </c>
+      <c r="B97" t="s" s="1332">
+        <v>397</v>
+      </c>
       <c r="C97" s="678" t="s">
         <v>17</v>
       </c>
@@ -5954,6 +7445,9 @@
       <c r="A98" s="110" t="s">
         <v>103</v>
       </c>
+      <c r="B98" t="s" s="1334">
+        <v>399</v>
+      </c>
       <c r="C98" s="680" t="s">
         <v>17</v>
       </c>
@@ -5962,6 +7456,9 @@
       <c r="A99" s="111" t="s">
         <v>104</v>
       </c>
+      <c r="B99" t="s" s="1336">
+        <v>401</v>
+      </c>
       <c r="C99" s="682" t="s">
         <v>17</v>
       </c>
@@ -5970,6 +7467,9 @@
       <c r="A100" s="112" t="s">
         <v>105</v>
       </c>
+      <c r="B100" t="s" s="1338">
+        <v>403</v>
+      </c>
       <c r="C100" s="684" t="s">
         <v>17</v>
       </c>
@@ -5978,6 +7478,9 @@
       <c r="A101" s="113" t="s">
         <v>106</v>
       </c>
+      <c r="B101" t="s" s="1340">
+        <v>405</v>
+      </c>
       <c r="C101" s="686" t="s">
         <v>17</v>
       </c>
@@ -5986,6 +7489,9 @@
       <c r="A102" s="114" t="s">
         <v>107</v>
       </c>
+      <c r="B102" t="s" s="1342">
+        <v>407</v>
+      </c>
       <c r="C102" s="688" t="s">
         <v>17</v>
       </c>
@@ -5994,6 +7500,9 @@
       <c r="A103" s="115" t="s">
         <v>108</v>
       </c>
+      <c r="B103" t="s" s="1344">
+        <v>409</v>
+      </c>
       <c r="C103" s="690" t="s">
         <v>17</v>
       </c>
@@ -6002,6 +7511,9 @@
       <c r="A104" s="116" t="s">
         <v>109</v>
       </c>
+      <c r="B104" t="s" s="1346">
+        <v>411</v>
+      </c>
       <c r="C104" s="692" t="s">
         <v>17</v>
       </c>
@@ -6010,6 +7522,9 @@
       <c r="A105" s="117" t="s">
         <v>110</v>
       </c>
+      <c r="B105" t="s" s="1348">
+        <v>412</v>
+      </c>
       <c r="C105" s="694" t="s">
         <v>17</v>
       </c>
@@ -6018,6 +7533,9 @@
       <c r="A106" s="118" t="s">
         <v>111</v>
       </c>
+      <c r="B106" t="s" s="1350">
+        <v>414</v>
+      </c>
       <c r="C106" s="696" t="s">
         <v>17</v>
       </c>
@@ -6026,6 +7544,9 @@
       <c r="A107" s="119" t="s">
         <v>112</v>
       </c>
+      <c r="B107" t="s" s="1352">
+        <v>426</v>
+      </c>
       <c r="C107" s="698" t="s">
         <v>17</v>
       </c>
@@ -6034,6 +7555,9 @@
       <c r="A108" s="120" t="s">
         <v>113</v>
       </c>
+      <c r="B108" t="s" s="1354">
+        <v>427</v>
+      </c>
       <c r="C108" s="700" t="s">
         <v>17</v>
       </c>
@@ -6042,6 +7566,9 @@
       <c r="A109" s="121" t="s">
         <v>114</v>
       </c>
+      <c r="B109" t="s" s="1356">
+        <v>428</v>
+      </c>
       <c r="C109" s="702" t="s">
         <v>17</v>
       </c>
@@ -6050,6 +7577,9 @@
       <c r="A110" s="122" t="s">
         <v>115</v>
       </c>
+      <c r="B110" t="s" s="1358">
+        <v>429</v>
+      </c>
       <c r="C110" s="704" t="s">
         <v>17</v>
       </c>
@@ -6058,6 +7588,9 @@
       <c r="A111" s="123" t="s">
         <v>116</v>
       </c>
+      <c r="B111" t="s" s="1360">
+        <v>428</v>
+      </c>
       <c r="C111" s="706" t="s">
         <v>17</v>
       </c>
@@ -6066,6 +7599,9 @@
       <c r="A112" s="124" t="s">
         <v>117</v>
       </c>
+      <c r="B112" t="s" s="1362">
+        <v>428</v>
+      </c>
       <c r="C112" s="708" t="s">
         <v>17</v>
       </c>
@@ -8912,6 +10448,1016 @@
     <row r="637">
       <c r="A637" t="s" s="1011">
         <v>350</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="s" s="1013">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="s" s="1014">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="s" s="1015">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="s" s="1016">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="s" s="1017">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="s" s="1018">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="s" s="1019">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="s" s="1021">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="s" s="1023">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="s" s="1025">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="s" s="1027">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="s" s="1029">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="s" s="1031">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="s" s="1033">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="s" s="1035">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="s" s="1037">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="s" s="1039">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="s" s="1041">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="s" s="1043">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="s" s="1045">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="s" s="1047">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="s" s="1049">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="s" s="1051">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="s" s="1053">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="s" s="1055">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="s" s="1057">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="s" s="1059">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="s" s="1061">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="s" s="1063">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="s" s="1065">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="s" s="1067">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="s" s="1069">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="s" s="1071">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="s" s="1073">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="s" s="1075">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="s" s="1077">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="s" s="1079">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="s" s="1081">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="s" s="1083">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="s" s="1085">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="s" s="1087">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="s" s="1089">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="s" s="1091">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="s" s="1093">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="s" s="1095">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="s" s="1097">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="s" s="1099">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="s" s="1101">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="s" s="1103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="s" s="1105">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="s" s="1107">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="s" s="1109">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="s" s="1111">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="s" s="1113">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="s" s="1115">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="s" s="1117">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="s" s="1119">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="s" s="1121">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="s" s="1123">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="s" s="1125">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="s" s="1127">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="s" s="1129">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="s" s="1131">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="s" s="1132">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="s" s="1133">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="s" s="1134">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="s" s="1135">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="s" s="1136">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="s" s="1137">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="s" s="1138">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="s" s="1139">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="s" s="1140">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="s" s="1141">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="s" s="1142">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="s" s="1143">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="s" s="1144">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="s" s="1145">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="s" s="1146">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="s" s="1147">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="s" s="1148">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="s" s="1149">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="s" s="1150">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="s" s="1151">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="s" s="1152">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="s" s="1153">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="s" s="1154">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="s" s="1155">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="s" s="1157">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="s" s="1159">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="s" s="1161">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="s" s="1163">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="s" s="1165">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="s" s="1167">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="s" s="1169">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="s" s="1171">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="s" s="1173">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="s" s="1175">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="s" s="1177">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="s" s="1179">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="s" s="1181">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="s" s="1183">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="s" s="1185">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="s" s="1187">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="s" s="1189">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="s" s="1191">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="s" s="1193">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="s" s="1195">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="s" s="1197">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="s" s="1199">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="s" s="1201">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="s" s="1203">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="s" s="1205">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="s" s="1206">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="s" s="1207">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="s" s="1208">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="s" s="1209">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="s" s="1210">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="s" s="1211">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="s" s="1212">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="s" s="1213">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="s" s="1214">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="s" s="1215">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="s" s="1216">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="s" s="1217">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="s" s="1218">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="s" s="1219">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="s" s="1220">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="s" s="1221">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="s" s="1222">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="s" s="1223">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="s" s="1224">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="s" s="1225">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="s" s="1226">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="s" s="1227">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="s" s="1228">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="s" s="1229">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="s" s="1231">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="s" s="1233">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="s" s="1235">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="s" s="1237">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="s" s="1239">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="s" s="1241">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="s" s="1243">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="s" s="1245">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="s" s="1247">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="s" s="1249">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="s" s="1251">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="s" s="1253">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="s" s="1255">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="s" s="1257">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="s" s="1259">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="s" s="1261">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="s" s="1263">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="s" s="1265">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="s" s="1267">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="s" s="1269">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="s" s="1271">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="s" s="1273">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="s" s="1275">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="s" s="1277">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="s" s="1279">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="s" s="1281">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="s" s="1283">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="s" s="1285">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="s" s="1287">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="s" s="1289">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="s" s="1291">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="s" s="1293">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="s" s="1295">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="s" s="1297">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="s" s="1299">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="s" s="1301">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="s" s="1303">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="s" s="1305">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="s" s="1307">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="s" s="1309">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="s" s="1311">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="s" s="1313">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="s" s="1315">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="s" s="1317">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="s" s="1319">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="s" s="1321">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="s" s="1323">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="s" s="1325">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="s" s="1327">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="s" s="1329">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="s" s="1331">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="s" s="1333">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="s" s="1335">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="s" s="1337">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="s" s="1339">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="s" s="1341">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="s" s="1343">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="s" s="1345">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="s" s="1347">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="s" s="1349">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="s" s="1351">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="s" s="1353">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="s" s="1355">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="s" s="1357">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="s" s="1359">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="s" s="1361">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IBH add create about, contact, tok page and delete articles
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/outputArticles.xlsx
+++ b/src/test/resources/testdata/outputArticles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850"/>
+    <workbookView windowWidth="21600" windowHeight="17250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -45,22 +45,25 @@
     <t>status</t>
   </si>
   <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/196</t>
-  </si>
-  <si>
-    <t>/samples-list</t>
-  </si>
-  <si>
     <t>https://yeti-cms.dev/yeti/main/articles/edit/197</t>
   </si>
   <si>
-    <t>/sample-hien</t>
+    <t>about-hien</t>
   </si>
   <si>
     <t>https://yeti-cms.dev/yeti/main/articles/edit/198</t>
   </si>
   <si>
+    <t>tokpage-hien</t>
+  </si>
+  <si>
     <t>https://yeti-cms.dev/yeti/main/articles/edit/199</t>
+  </si>
+  <si>
+    <t>contacts-hien</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
   <si>
     <t>https://yeti-cms.dev/yeti/main/articles/edit/200</t>
@@ -69,463 +72,7 @@
     <t>https://yeti-cms.dev/yeti/main/articles/edit/201</t>
   </si>
   <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/298</t>
-  </si>
-  <si>
-    <t>/samples/essay/gender-studies</t>
-  </si>
-  <si>
     <t>https://yeti-cms.dev/yeti/main/articles/edit/202</t>
-  </si>
-  <si>
-    <t>/sample-test</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/220</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/221</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/222</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/223</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/224</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/225</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/226</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/227</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/228</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/229</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/230</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/231</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/232</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/233</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/234</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/235</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/236</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/237</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/238</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/239</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/240</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/241</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/242</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/writers/edit/243</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/268</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/269</t>
-  </si>
-  <si>
-    <t>/samples/essay/persuasive-essay</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/270</t>
-  </si>
-  <si>
-    <t>/samples/essay/mba-application</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/271</t>
-  </si>
-  <si>
-    <t>/samples/essay/anthropology</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/272</t>
-  </si>
-  <si>
-    <t>/samples/essay/criminal-law</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/273</t>
-  </si>
-  <si>
-    <t>/samples/discussion-post/health-care</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/274</t>
-  </si>
-  <si>
-    <t>/discussion-post/history</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/275</t>
-  </si>
-  <si>
-    <t>/samples/discussion-post/statistics</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/276</t>
-  </si>
-  <si>
-    <t>/samples/critical-thinking/criminal-law</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/277</t>
-  </si>
-  <si>
-    <t>/samples/critical-thinking/culture-and-society</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/278</t>
-  </si>
-  <si>
-    <t>/samples/term-paper/criminal-law</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/279</t>
-  </si>
-  <si>
-    <t>/samples/homework/statistics</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/280</t>
-  </si>
-  <si>
-    <t>/samples/research-paper/apa</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/281</t>
-  </si>
-  <si>
-    <t>/samples/research-paper/gun-control</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/282</t>
-  </si>
-  <si>
-    <t>/samples/research-paper/business-managment</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/283</t>
-  </si>
-  <si>
-    <t>/samples/research-proposal/phd</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/284</t>
-  </si>
-  <si>
-    <t>/samples/research-proposal/mla</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/285</t>
-  </si>
-  <si>
-    <t>/samples/personal-statement/medicine</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/286</t>
-  </si>
-  <si>
-    <t>/samples/powerpoint-presentation/powerpoint-presentation-apa</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/287</t>
-  </si>
-  <si>
-    <t>/samples/speech/graduation</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/288</t>
-  </si>
-  <si>
-    <t>/samples/speech/high-school</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/289</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/spectrophotometry-lab</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/290</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/chemistry</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/291</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/physics</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/292</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/biology</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/293</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/statistics</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/294</t>
-  </si>
-  <si>
-    <t>/samples/lesson-plan/education</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/295</t>
-  </si>
-  <si>
-    <t>/samples/nursing-plan/nursing</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/296</t>
-  </si>
-  <si>
-    <t>/samples/epq-essay/essay</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/297</t>
-  </si>
-  <si>
-    <t>/samples/epq-presentation/presentation</t>
-  </si>
-  <si>
-    <t>/samples/question-answer/psychology</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/190</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/191</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/192</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/346</t>
-  </si>
-  <si>
-    <t>/samples/essay/gender-studies5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/348</t>
-  </si>
-  <si>
-    <t>/samples/essay/persuasive-essay5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/350</t>
-  </si>
-  <si>
-    <t>/samples/essay/mba-application5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/352</t>
-  </si>
-  <si>
-    <t>/samples/essay/anthropology5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/354</t>
-  </si>
-  <si>
-    <t>/samples/essay/criminal-law5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/355</t>
-  </si>
-  <si>
-    <t>/samples/discussion-post/health-care5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/357</t>
-  </si>
-  <si>
-    <t>/discussion-post/history5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/359</t>
-  </si>
-  <si>
-    <t>/samples/discussion-post/statistics5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/361</t>
-  </si>
-  <si>
-    <t>/samples/critical-thinking/criminal-law5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/363</t>
-  </si>
-  <si>
-    <t>/samples/critical-thinking/culture-and-society5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/365</t>
-  </si>
-  <si>
-    <t>/samples/term-paper/criminal-law5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/367</t>
-  </si>
-  <si>
-    <t>/samples/homework/statistics5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/369</t>
-  </si>
-  <si>
-    <t>/samples/research-paper/apa5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/371</t>
-  </si>
-  <si>
-    <t>/samples/research-paper/gun-control5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/372</t>
-  </si>
-  <si>
-    <t>/samples/research-paper/business-managment5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/374</t>
-  </si>
-  <si>
-    <t>/samples/research-proposal/phd5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/376</t>
-  </si>
-  <si>
-    <t>/samples/research-proposal/mla5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/378</t>
-  </si>
-  <si>
-    <t>/samples/personal-statement/medicine5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/380</t>
-  </si>
-  <si>
-    <t>/samples/powerpoint-presentation/powerpoint-presentation-apa5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/382</t>
-  </si>
-  <si>
-    <t>/samples/speech/graduation5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/384</t>
-  </si>
-  <si>
-    <t>/samples/speech/high-school5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/386</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/spectrophotometry-lab5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/388</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/chemistry5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/390</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/physics5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/392</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/biology5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/394</t>
-  </si>
-  <si>
-    <t>/samples/lab-report/statistics5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/396</t>
-  </si>
-  <si>
-    <t>/samples/lesson-plan/education5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/398</t>
-  </si>
-  <si>
-    <t>/samples/nursing-plan/nursing5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/400</t>
-  </si>
-  <si>
-    <t>/samples/epq-essay/essay5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/402</t>
-  </si>
-  <si>
-    <t>/samples/epq-presentation/presentation5</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/samples/edit/403</t>
-  </si>
-  <si>
-    <t>/samples/question-answer/psychology5</t>
   </si>
 </sst>
 </file>
@@ -1169,493 +716,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
@@ -2004,10 +1068,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E839"/>
+  <dimension ref="A1:E835"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2034,827 +1098,517 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="9" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>8</v>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="11" t="s">
-        <v>11</v>
+      <c r="A6" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
-        <v>12</v>
+      <c r="A7" s="10" t="s">
+        <v>14</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>6</v>
+      <c r="B7" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>14</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>43</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>45</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>47</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>49</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="54" t="s">
-        <v>51</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>53</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="58" t="s">
-        <v>55</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>57</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>59</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="64" t="s">
-        <v>61</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="66" t="s">
-        <v>63</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="68" t="s">
-        <v>65</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="70" t="s">
-        <v>67</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="72" t="s">
-        <v>69</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="74" t="s">
-        <v>71</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="76" t="s">
-        <v>73</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="78" t="s">
-        <v>75</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="80" t="s">
-        <v>77</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="82" t="s">
-        <v>79</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="84" t="s">
-        <v>81</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="86" t="s">
-        <v>83</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="88" t="s">
-        <v>85</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="90" t="s">
-        <v>87</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="92" t="s">
-        <v>89</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="94" t="s">
-        <v>91</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="96" t="s">
-        <v>93</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="98" t="s">
-        <v>95</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="100" t="s">
-        <v>97</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="102" t="s">
-        <v>99</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="104" t="s">
-        <v>100</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="106" t="s">
-        <v>8</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="108" t="s">
-        <v>6</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="110" t="s">
-        <v>16</v>
-      </c>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="112" t="s">
-        <v>105</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" s="114" t="s">
-        <v>107</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="116" t="s">
-        <v>109</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" s="118" t="s">
-        <v>111</v>
-      </c>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" s="120" t="s">
-        <v>113</v>
-      </c>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" s="122" t="s">
-        <v>115</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="B50" s="124" t="s">
-        <v>117</v>
-      </c>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="126" t="s">
-        <v>119</v>
-      </c>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="79" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="128" t="s">
-        <v>121</v>
-      </c>
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="130" t="s">
-        <v>123</v>
-      </c>
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="83" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" s="132" t="s">
-        <v>125</v>
-      </c>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="134" t="s">
-        <v>127</v>
-      </c>
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="136" t="s">
-        <v>129</v>
-      </c>
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="89" t="s">
-        <v>86</v>
-      </c>
-      <c r="B57" s="138" t="s">
-        <v>131</v>
-      </c>
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" s="140" t="s">
-        <v>133</v>
-      </c>
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="93" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="142" t="s">
-        <v>135</v>
-      </c>
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="95" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="144" t="s">
-        <v>137</v>
-      </c>
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="97" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61" s="146" t="s">
-        <v>139</v>
-      </c>
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="99" t="s">
-        <v>96</v>
-      </c>
-      <c r="B62" s="148" t="s">
-        <v>141</v>
-      </c>
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="101" t="s">
-        <v>98</v>
-      </c>
-      <c r="B63" s="150" t="s">
-        <v>143</v>
-      </c>
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="103" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" s="152" t="s">
-        <v>145</v>
-      </c>
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="105" t="s">
-        <v>101</v>
-      </c>
-      <c r="B65" s="154" t="s">
-        <v>147</v>
-      </c>
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="107" t="s">
-        <v>102</v>
-      </c>
-      <c r="B66" s="156" t="s">
-        <v>149</v>
-      </c>
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="109" t="s">
-        <v>103</v>
-      </c>
-      <c r="B67" s="158" t="s">
-        <v>151</v>
-      </c>
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="111" t="s">
-        <v>104</v>
-      </c>
-      <c r="B68" s="160" t="s">
-        <v>153</v>
-      </c>
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="113" t="s">
-        <v>106</v>
-      </c>
-      <c r="B69" s="162" t="s">
-        <v>155</v>
-      </c>
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="115" t="s">
-        <v>108</v>
-      </c>
-      <c r="B70" s="164" t="s">
-        <v>157</v>
-      </c>
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
       <c r="C70" s="2"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="117" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" s="166" t="s">
-        <v>159</v>
-      </c>
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
       <c r="C71" s="2"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="119" t="s">
-        <v>112</v>
-      </c>
-      <c r="B72" s="168" t="s">
-        <v>161</v>
-      </c>
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
       <c r="C72" s="2"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="121" t="s">
-        <v>114</v>
-      </c>
-      <c r="B73" s="170" t="s">
-        <v>163</v>
-      </c>
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
       <c r="C73" s="2"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="123" t="s">
-        <v>116</v>
-      </c>
-      <c r="B74" s="172" t="s">
-        <v>165</v>
-      </c>
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
       <c r="C74" s="2"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="125" t="s">
-        <v>118</v>
-      </c>
+      <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="127" t="s">
-        <v>120</v>
-      </c>
+      <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="129" t="s">
-        <v>122</v>
-      </c>
+      <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="131" t="s">
-        <v>124</v>
-      </c>
+      <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="133" t="s">
-        <v>126</v>
-      </c>
+      <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="135" t="s">
-        <v>128</v>
-      </c>
+      <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="137" t="s">
-        <v>130</v>
-      </c>
+      <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="139" t="s">
-        <v>132</v>
-      </c>
+      <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="141" t="s">
-        <v>134</v>
-      </c>
+      <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="143" t="s">
-        <v>136</v>
-      </c>
+      <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="145" t="s">
-        <v>138</v>
-      </c>
+      <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="147" t="s">
-        <v>140</v>
-      </c>
+      <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="149" t="s">
-        <v>142</v>
-      </c>
+      <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="151" t="s">
-        <v>144</v>
-      </c>
+      <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="153" t="s">
-        <v>146</v>
-      </c>
+      <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="155" t="s">
-        <v>148</v>
-      </c>
+      <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="157" t="s">
-        <v>150</v>
-      </c>
+      <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="159" t="s">
-        <v>152</v>
-      </c>
+      <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="161" t="s">
-        <v>154</v>
-      </c>
+      <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="163" t="s">
-        <v>156</v>
-      </c>
+      <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="165" t="s">
-        <v>158</v>
-      </c>
+      <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="167" t="s">
-        <v>160</v>
-      </c>
+      <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="169" t="s">
-        <v>162</v>
-      </c>
+      <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="171" t="s">
-        <v>164</v>
-      </c>
+      <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
     </row>
@@ -2910,22 +1664,18 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
       <c r="C110" s="2"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
       <c r="C111" s="2"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
       <c r="C112" s="2"/>
     </row>
     <row r="113" spans="1:3">
@@ -3204,21 +1954,17 @@
       <c r="A181" s="2"/>
       <c r="C181" s="2"/>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:1">
       <c r="A182" s="2"/>
-      <c r="C182" s="2"/>
-    </row>
-    <row r="183" spans="1:3">
+    </row>
+    <row r="183" spans="1:1">
       <c r="A183" s="2"/>
-      <c r="C183" s="2"/>
-    </row>
-    <row r="184" spans="1:3">
+    </row>
+    <row r="184" spans="1:1">
       <c r="A184" s="2"/>
-      <c r="C184" s="2"/>
-    </row>
-    <row r="185" spans="1:3">
+    </row>
+    <row r="185" spans="1:1">
       <c r="A185" s="2"/>
-      <c r="C185" s="2"/>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="2"/>
@@ -5169,18 +3915,6 @@
     </row>
     <row r="835" spans="1:1">
       <c r="A835" s="2"/>
-    </row>
-    <row r="836" spans="1:1">
-      <c r="A836" s="2"/>
-    </row>
-    <row r="837" spans="1:1">
-      <c r="A837" s="2"/>
-    </row>
-    <row r="838" spans="1:1">
-      <c r="A838" s="2"/>
-    </row>
-    <row r="839" spans="1:1">
-      <c r="A839" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update createWriterReviewWPH and fixbug
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/outputArticles.xlsx
+++ b/src/test/resources/testdata/outputArticles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18360"/>
+    <workbookView windowWidth="28000" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -32,43 +32,328 @@
     <t>status</t>
   </si>
   <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/189</t>
-  </si>
-  <si>
-    <t>about-hien</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/190</t>
-  </si>
-  <si>
-    <t>vy</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/191</t>
-  </si>
-  <si>
-    <t>Aboutvy2</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/192</t>
-  </si>
-  <si>
-    <t>About-vy3</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/193</t>
-  </si>
-  <si>
-    <t>about</t>
-  </si>
-  <si>
-    <t>tokpage1</t>
-  </si>
-  <si>
-    <t>https://yeti-cms.dev/yeti/main/articles/edit/195</t>
-  </si>
-  <si>
-    <t>/TokPageTest</t>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/242</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/243</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/244</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/245</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/246</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/247</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/248</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/249</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/250</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/251</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/252</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/253</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/255</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/256</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/257</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/259</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/260</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/261</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/262</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/263</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/264</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/265</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/266</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/267</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/268</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/269</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/270</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/271</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/272</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/273</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/274</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/275</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/276</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/277</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/278</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/279</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/280</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/281</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/282</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/283</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/284</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/285</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/286</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/287</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/288</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/289</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/290</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/291</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/292</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/293</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/294</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/295</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/296</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/297</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/298</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/299</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/300</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/301</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/302</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/303</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/304</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/305</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/306</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/307</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/308</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/309</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/310</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/311</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/312</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/313</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/314</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/315</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/316</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/317</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/318</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/319</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/320</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/321</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/322</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/323</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/324</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/325</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/326</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/327</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/328</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/329</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/330</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/331</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/332</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/333</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/334</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/335</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/336</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/337</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/338</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/339</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/340</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/341</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/342</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/343</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/344</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/345</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/346</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/347</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/348</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/349</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/350</t>
+  </si>
+  <si>
+    <t>https://yeti-cms.dev/yeti/main/writers/edit/351</t>
   </si>
 </sst>
 </file>
@@ -76,10 +361,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -96,9 +381,107 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,34 +495,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,9 +503,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,79 +519,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -255,7 +540,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,7 +558,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,19 +588,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +612,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +660,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,31 +696,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,73 +720,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,17 +752,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,7 +765,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,21 +786,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -531,6 +795,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -547,6 +826,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -555,167 +849,443 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
@@ -1079,7 +1649,7 @@
   <dimension ref="A1:E835"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1089,11 +1659,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>17</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1106,542 +1676,758 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2"/>
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="2"/>
+      <c r="A19" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="2"/>
+      <c r="A20" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="2"/>
+      <c r="A21" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2"/>
+      <c r="A22" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="2"/>
+      <c r="A23" s="24" t="s">
+        <v>26</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="2"/>
+      <c r="A25" s="26" t="s">
+        <v>28</v>
+      </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2"/>
+      <c r="A26" s="27" t="s">
+        <v>29</v>
+      </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2"/>
+      <c r="A27" s="28" t="s">
+        <v>30</v>
+      </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="2"/>
+      <c r="A28" s="29" t="s">
+        <v>31</v>
+      </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="2"/>
+      <c r="A29" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="2"/>
+      <c r="A30" s="31" t="s">
+        <v>33</v>
+      </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="2"/>
+      <c r="A31" s="32" t="s">
+        <v>34</v>
+      </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2"/>
+      <c r="A32" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="2"/>
+      <c r="A33" s="34" t="s">
+        <v>36</v>
+      </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2"/>
+      <c r="A34" s="35" t="s">
+        <v>37</v>
+      </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="2"/>
+      <c r="A35" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2"/>
+      <c r="A36" s="37" t="s">
+        <v>39</v>
+      </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2"/>
+      <c r="A37" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2"/>
+      <c r="A38" s="39" t="s">
+        <v>41</v>
+      </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2"/>
+      <c r="A39" s="40" t="s">
+        <v>42</v>
+      </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="2"/>
+      <c r="A40" s="41" t="s">
+        <v>43</v>
+      </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2"/>
+      <c r="A41" s="42" t="s">
+        <v>44</v>
+      </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="2"/>
+      <c r="A42" s="43" t="s">
+        <v>45</v>
+      </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="2"/>
+      <c r="A43" s="44" t="s">
+        <v>46</v>
+      </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2"/>
+      <c r="A44" s="45" t="s">
+        <v>47</v>
+      </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2"/>
+      <c r="A45" s="46" t="s">
+        <v>48</v>
+      </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2"/>
+      <c r="A46" s="47" t="s">
+        <v>49</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="2"/>
+      <c r="A47" s="48" t="s">
+        <v>50</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="2"/>
+      <c r="A48" s="49" t="s">
+        <v>51</v>
+      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="2"/>
+      <c r="A49" s="50" t="s">
+        <v>52</v>
+      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="2"/>
+      <c r="A50" s="51" t="s">
+        <v>53</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2"/>
+      <c r="A51" s="52" t="s">
+        <v>54</v>
+      </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="2"/>
+      <c r="A52" s="53" t="s">
+        <v>55</v>
+      </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="2"/>
+      <c r="A53" s="54" t="s">
+        <v>56</v>
+      </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="2"/>
+      <c r="A54" s="55" t="s">
+        <v>57</v>
+      </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="2"/>
+      <c r="A55" s="56" t="s">
+        <v>58</v>
+      </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="2"/>
+      <c r="A56" s="57" t="s">
+        <v>59</v>
+      </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="2"/>
+      <c r="A57" s="58" t="s">
+        <v>60</v>
+      </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="2"/>
+      <c r="A58" s="59" t="s">
+        <v>61</v>
+      </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="2"/>
+      <c r="A59" s="60" t="s">
+        <v>62</v>
+      </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="2"/>
+      <c r="A60" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="2"/>
+      <c r="A61" s="62" t="s">
+        <v>64</v>
+      </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="2"/>
+      <c r="A62" s="63" t="s">
+        <v>65</v>
+      </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="2"/>
+      <c r="A63" s="64" t="s">
+        <v>66</v>
+      </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="2"/>
+      <c r="A64" s="65" t="s">
+        <v>67</v>
+      </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="2"/>
+      <c r="A65" s="66" t="s">
+        <v>68</v>
+      </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="2"/>
+      <c r="A66" s="67" t="s">
+        <v>69</v>
+      </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="2"/>
+      <c r="A67" s="68" t="s">
+        <v>70</v>
+      </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="2"/>
+      <c r="A68" s="69" t="s">
+        <v>71</v>
+      </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="2"/>
+      <c r="A69" s="70" t="s">
+        <v>72</v>
+      </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="2"/>
+      <c r="A70" s="71" t="s">
+        <v>73</v>
+      </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="2"/>
+      <c r="A71" s="72" t="s">
+        <v>74</v>
+      </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="2"/>
+      <c r="A72" s="73" t="s">
+        <v>75</v>
+      </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="2"/>
+      <c r="A73" s="74" t="s">
+        <v>76</v>
+      </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="2"/>
+      <c r="A74" s="75" t="s">
+        <v>77</v>
+      </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="2"/>
+      <c r="A75" s="76" t="s">
+        <v>78</v>
+      </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="2"/>
+      <c r="A76" s="77" t="s">
+        <v>79</v>
+      </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="2"/>
+      <c r="A77" s="78" t="s">
+        <v>80</v>
+      </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="2"/>
+      <c r="A78" s="79" t="s">
+        <v>81</v>
+      </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="2"/>
+      <c r="A79" s="80" t="s">
+        <v>82</v>
+      </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="2"/>
+      <c r="A80" s="81" t="s">
+        <v>83</v>
+      </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="2"/>
+      <c r="A81" s="82" t="s">
+        <v>84</v>
+      </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="2"/>
+      <c r="A82" s="83" t="s">
+        <v>85</v>
+      </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="2"/>
+      <c r="A83" s="84" t="s">
+        <v>86</v>
+      </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="2"/>
+      <c r="A84" s="85" t="s">
+        <v>87</v>
+      </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="2"/>
+      <c r="A85" s="86" t="s">
+        <v>88</v>
+      </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="2"/>
+      <c r="A86" s="87" t="s">
+        <v>89</v>
+      </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="2"/>
+      <c r="A87" s="88" t="s">
+        <v>90</v>
+      </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="2"/>
+      <c r="A88" s="89" t="s">
+        <v>91</v>
+      </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="2"/>
+      <c r="A89" s="90" t="s">
+        <v>92</v>
+      </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="2"/>
+      <c r="A90" s="91" t="s">
+        <v>93</v>
+      </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="2"/>
+      <c r="A91" s="92" t="s">
+        <v>94</v>
+      </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="2"/>
+      <c r="A92" s="93" t="s">
+        <v>95</v>
+      </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="2"/>
+      <c r="A93" s="94" t="s">
+        <v>96</v>
+      </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="2"/>
+      <c r="A94" s="95" t="s">
+        <v>97</v>
+      </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="2"/>
+      <c r="A95" s="96" t="s">
+        <v>98</v>
+      </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="2"/>
+      <c r="A96" s="97" t="s">
+        <v>99</v>
+      </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="2"/>
+      <c r="A97" s="98" t="s">
+        <v>100</v>
+      </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="2"/>
+      <c r="A98" s="99" t="s">
+        <v>101</v>
+      </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="2"/>
+      <c r="A99" s="100" t="s">
+        <v>102</v>
+      </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="2"/>
+      <c r="A100" s="101" t="s">
+        <v>103</v>
+      </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="2"/>
+      <c r="A101" s="102" t="s">
+        <v>104</v>
+      </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="2"/>
+      <c r="A102" s="103" t="s">
+        <v>105</v>
+      </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="2"/>
+      <c r="A103" s="104" t="s">
+        <v>106</v>
+      </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="2"/>
+      <c r="A104" s="105" t="s">
+        <v>107</v>
+      </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="2"/>
+      <c r="A105" s="106" t="s">
+        <v>108</v>
+      </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="2"/>
+      <c r="A106" s="107" t="s">
+        <v>109</v>
+      </c>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="2"/>
+      <c r="A107" s="108" t="s">
+        <v>110</v>
+      </c>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="2"/>
+      <c r="A108" s="109" t="s">
+        <v>111</v>
+      </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="2"/>
+      <c r="A109" s="110" t="s">
+        <v>112</v>
+      </c>
       <c r="C109" s="2"/>
     </row>
     <row r="110" spans="1:3">
@@ -3906,7 +4692,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>

</xml_diff>